<commit_message>
Added Chapter Four Labs
</commit_message>
<xml_diff>
--- a/ANOVA Practice.xlsx
+++ b/ANOVA Practice.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="100" windowWidth="19100" windowHeight="7300" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="100" windowWidth="19100" windowHeight="7300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ANOVA SHEET" sheetId="1" r:id="rId1"/>
     <sheet name="MULTICOLLINEARITY SHEET" sheetId="2" r:id="rId2"/>
     <sheet name="POST-HOC TEST" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="85">
   <si>
     <t>Normal</t>
   </si>
@@ -259,15 +260,28 @@
   </si>
   <si>
     <t>Total number of groups divided by the degree of freedom of observation from the three groups</t>
+  </si>
+  <si>
+    <t>X Norm</t>
+  </si>
+  <si>
+    <t>Sorted X</t>
+  </si>
+  <si>
+    <t>Normal X</t>
+  </si>
+  <si>
+    <t>x - mean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -311,12 +325,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="25">
@@ -635,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -766,6 +786,19 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1710,8 +1743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AG51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4298,4 +4331,1070 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="D3:N31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31:N31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="9" max="9" width="10.54296875" customWidth="1"/>
+    <col min="10" max="10" width="11.08984375" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" customWidth="1"/>
+    <col min="12" max="12" width="12.1796875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:14" ht="15">
+      <c r="E3" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="M3" s="33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="4:14" ht="15">
+      <c r="D4" s="48">
+        <v>1</v>
+      </c>
+      <c r="E4" s="35">
+        <v>13.6</v>
+      </c>
+      <c r="F4" s="35">
+        <v>14.1</v>
+      </c>
+      <c r="G4" s="35">
+        <v>0.86</v>
+      </c>
+      <c r="H4" s="35">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="I4" s="35">
+        <v>14.1</v>
+      </c>
+      <c r="J4" s="35">
+        <v>1</v>
+      </c>
+      <c r="K4" s="35">
+        <f>SUM((J4-12.22)/28.2)</f>
+        <v>-0.39787234042553193</v>
+      </c>
+      <c r="L4" s="50">
+        <f>SUM(K4*K4)</f>
+        <v>0.15830239927569037</v>
+      </c>
+      <c r="M4" s="35">
+        <f>SUM(J4-12.22)</f>
+        <v>-11.22</v>
+      </c>
+      <c r="N4">
+        <f>SUM(M4*M4)</f>
+        <v>125.88840000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="4:14" ht="15">
+      <c r="D5" s="48">
+        <v>2</v>
+      </c>
+      <c r="E5" s="35">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="F5" s="35">
+        <v>16</v>
+      </c>
+      <c r="G5" s="35">
+        <v>1.06</v>
+      </c>
+      <c r="H5" s="35">
+        <v>1.093</v>
+      </c>
+      <c r="I5" s="35">
+        <v>16</v>
+      </c>
+      <c r="J5" s="35">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="K5" s="35">
+        <f t="shared" ref="K5:K28" si="0">SUM((J5-12.22)/28.2)</f>
+        <v>-0.28794326241134754</v>
+      </c>
+      <c r="L5" s="50">
+        <f t="shared" ref="L5:L28" si="1">SUM(K5*K5)</f>
+        <v>8.2911322368090151E-2</v>
+      </c>
+      <c r="M5" s="35">
+        <f t="shared" ref="M5:M28" si="2">SUM(J5-12.22)</f>
+        <v>-8.120000000000001</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N5:N28" si="3">SUM(M5*M5)</f>
+        <v>65.934400000000011</v>
+      </c>
+    </row>
+    <row r="6" spans="4:14" ht="15">
+      <c r="D6" s="48">
+        <v>3</v>
+      </c>
+      <c r="E6" s="35">
+        <v>23.5</v>
+      </c>
+      <c r="F6" s="35">
+        <v>29.8</v>
+      </c>
+      <c r="G6" s="35">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="H6" s="35">
+        <v>1.165</v>
+      </c>
+      <c r="I6" s="35">
+        <v>29.8</v>
+      </c>
+      <c r="J6" s="35">
+        <v>4.5</v>
+      </c>
+      <c r="K6" s="35">
+        <f t="shared" si="0"/>
+        <v>-0.27375886524822696</v>
+      </c>
+      <c r="L6" s="50">
+        <f t="shared" si="1"/>
+        <v>7.4943916301996885E-2</v>
+      </c>
+      <c r="M6" s="35">
+        <f t="shared" si="2"/>
+        <v>-7.7200000000000006</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="3"/>
+        <v>59.598400000000012</v>
+      </c>
+    </row>
+    <row r="7" spans="4:14" ht="15">
+      <c r="D7" s="48">
+        <v>4</v>
+      </c>
+      <c r="E7" s="35">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="F7" s="35">
+        <v>8</v>
+      </c>
+      <c r="G7" s="35">
+        <v>0.67</v>
+      </c>
+      <c r="H7" s="35">
+        <v>0.92</v>
+      </c>
+      <c r="I7" s="35">
+        <v>8</v>
+      </c>
+      <c r="J7" s="35">
+        <v>7.3</v>
+      </c>
+      <c r="K7" s="35">
+        <f t="shared" si="0"/>
+        <v>-0.17446808510638301</v>
+      </c>
+      <c r="L7" s="50">
+        <f t="shared" si="1"/>
+        <v>3.0439112720688104E-2</v>
+      </c>
+      <c r="M7" s="35">
+        <f t="shared" si="2"/>
+        <v>-4.9200000000000008</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="3"/>
+        <v>24.206400000000009</v>
+      </c>
+    </row>
+    <row r="8" spans="4:14" ht="15">
+      <c r="D8" s="48">
+        <v>5</v>
+      </c>
+      <c r="E8" s="35">
+        <v>5.4</v>
+      </c>
+      <c r="F8" s="35">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G8" s="35">
+        <v>0.4</v>
+      </c>
+      <c r="H8" s="35">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="I8" s="35">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="J8" s="35">
+        <v>7.8</v>
+      </c>
+      <c r="K8" s="35">
+        <f t="shared" si="0"/>
+        <v>-0.1567375886524823</v>
+      </c>
+      <c r="L8" s="50">
+        <f t="shared" si="1"/>
+        <v>2.4566671696594749E-2</v>
+      </c>
+      <c r="M8" s="35">
+        <f t="shared" si="2"/>
+        <v>-4.4200000000000008</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="3"/>
+        <v>19.536400000000008</v>
+      </c>
+    </row>
+    <row r="9" spans="4:14" ht="15">
+      <c r="D9" s="48">
+        <v>6</v>
+      </c>
+      <c r="E9" s="35">
+        <v>15</v>
+      </c>
+      <c r="F9" s="35">
+        <v>15</v>
+      </c>
+      <c r="G9" s="35">
+        <v>1.04</v>
+      </c>
+      <c r="H9" s="35">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="I9" s="35">
+        <v>15</v>
+      </c>
+      <c r="J9" s="35">
+        <v>8</v>
+      </c>
+      <c r="K9" s="35">
+        <f t="shared" si="0"/>
+        <v>-0.14964539007092201</v>
+      </c>
+      <c r="L9" s="50">
+        <f t="shared" si="1"/>
+        <v>2.2393742769478402E-2</v>
+      </c>
+      <c r="M9" s="35">
+        <f t="shared" si="2"/>
+        <v>-4.2200000000000006</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="3"/>
+        <v>17.808400000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="4:14" ht="15">
+      <c r="D10" s="48">
+        <v>7</v>
+      </c>
+      <c r="E10" s="35">
+        <v>9</v>
+      </c>
+      <c r="F10" s="35">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G10" s="35">
+        <v>0.76</v>
+      </c>
+      <c r="H10" s="35">
+        <v>1.0269999999999999</v>
+      </c>
+      <c r="I10" s="35">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J10" s="35">
+        <v>8.6</v>
+      </c>
+      <c r="K10" s="35">
+        <f t="shared" si="0"/>
+        <v>-0.12836879432624118</v>
+      </c>
+      <c r="L10" s="50">
+        <f t="shared" si="1"/>
+        <v>1.6478547356772809E-2</v>
+      </c>
+      <c r="M10" s="35">
+        <f t="shared" si="2"/>
+        <v>-3.620000000000001</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="3"/>
+        <v>13.104400000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="4:14" ht="15">
+      <c r="D11" s="48">
+        <v>8</v>
+      </c>
+      <c r="E11" s="35">
+        <v>12.3</v>
+      </c>
+      <c r="F11" s="35">
+        <v>12.4</v>
+      </c>
+      <c r="G11" s="35">
+        <v>0.95</v>
+      </c>
+      <c r="H11" s="35">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="I11" s="35">
+        <v>12.4</v>
+      </c>
+      <c r="J11" s="35">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="K11" s="35">
+        <f t="shared" si="0"/>
+        <v>-0.12127659574468085</v>
+      </c>
+      <c r="L11" s="50">
+        <f t="shared" si="1"/>
+        <v>1.470801267541874E-2</v>
+      </c>
+      <c r="M11" s="35">
+        <f t="shared" si="2"/>
+        <v>-3.42</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="3"/>
+        <v>11.696399999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="4:14" ht="15">
+      <c r="D12" s="48">
+        <v>9</v>
+      </c>
+      <c r="E12" s="35">
+        <v>16.3</v>
+      </c>
+      <c r="F12" s="35">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="G12" s="35">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="H12" s="35">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="I12" s="35">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="J12" s="35">
+        <v>9</v>
+      </c>
+      <c r="K12" s="35">
+        <f t="shared" si="0"/>
+        <v>-0.11418439716312059</v>
+      </c>
+      <c r="L12" s="50">
+        <f t="shared" si="1"/>
+        <v>1.3038076555505262E-2</v>
+      </c>
+      <c r="M12" s="35">
+        <f t="shared" si="2"/>
+        <v>-3.2200000000000006</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="3"/>
+        <v>10.368400000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="4:14" ht="15">
+      <c r="D13" s="48">
+        <v>10</v>
+      </c>
+      <c r="E13" s="35">
+        <v>15.4</v>
+      </c>
+      <c r="F13" s="35">
+        <v>14.9</v>
+      </c>
+      <c r="G13" s="35">
+        <v>1.02</v>
+      </c>
+      <c r="H13" s="35">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="I13" s="35">
+        <v>14.9</v>
+      </c>
+      <c r="J13" s="35">
+        <v>11.4</v>
+      </c>
+      <c r="K13" s="35">
+        <f t="shared" si="0"/>
+        <v>-2.9078014184397174E-2</v>
+      </c>
+      <c r="L13" s="50">
+        <f t="shared" si="1"/>
+        <v>8.4553090890800327E-4</v>
+      </c>
+      <c r="M13" s="35">
+        <f t="shared" si="2"/>
+        <v>-0.82000000000000028</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="3"/>
+        <v>0.67240000000000044</v>
+      </c>
+    </row>
+    <row r="14" spans="4:14" ht="15">
+      <c r="D14" s="48">
+        <v>11</v>
+      </c>
+      <c r="E14" s="35">
+        <v>13</v>
+      </c>
+      <c r="F14" s="35">
+        <v>13.7</v>
+      </c>
+      <c r="G14" s="35">
+        <v>1.01</v>
+      </c>
+      <c r="H14" s="35">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="I14" s="35">
+        <v>13.7</v>
+      </c>
+      <c r="J14" s="35">
+        <v>12</v>
+      </c>
+      <c r="K14" s="35">
+        <f t="shared" si="0"/>
+        <v>-7.8014184397163346E-3</v>
+      </c>
+      <c r="L14" s="50">
+        <f t="shared" si="1"/>
+        <v>6.0862129671546051E-5</v>
+      </c>
+      <c r="M14" s="35">
+        <f t="shared" si="2"/>
+        <v>-0.22000000000000064</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="3"/>
+        <v>4.8400000000000283E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="4:14" ht="15">
+      <c r="D15" s="48">
+        <v>12</v>
+      </c>
+      <c r="E15" s="35">
+        <v>14</v>
+      </c>
+      <c r="F15" s="35">
+        <v>15.1</v>
+      </c>
+      <c r="G15" s="35">
+        <v>0.9</v>
+      </c>
+      <c r="H15" s="35">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="I15" s="35">
+        <v>15.1</v>
+      </c>
+      <c r="J15" s="35">
+        <v>12.4</v>
+      </c>
+      <c r="K15" s="35">
+        <f t="shared" si="0"/>
+        <v>6.3829787234042454E-3</v>
+      </c>
+      <c r="L15" s="50">
+        <f t="shared" si="1"/>
+        <v>4.0742417383431288E-5</v>
+      </c>
+      <c r="M15" s="35">
+        <f t="shared" si="2"/>
+        <v>0.17999999999999972</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="3"/>
+        <v>3.2399999999999901E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="4:14" ht="15">
+      <c r="D16" s="48">
+        <v>13</v>
+      </c>
+      <c r="E16" s="35">
+        <v>10</v>
+      </c>
+      <c r="F16" s="35">
+        <v>7.8</v>
+      </c>
+      <c r="G16" s="35">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H16" s="35">
+        <v>0.97</v>
+      </c>
+      <c r="I16" s="35">
+        <v>7.8</v>
+      </c>
+      <c r="J16" s="35">
+        <v>12.8</v>
+      </c>
+      <c r="K16" s="35">
+        <f t="shared" si="0"/>
+        <v>2.0567375886524825E-2</v>
+      </c>
+      <c r="L16" s="50">
+        <f t="shared" si="1"/>
+        <v>4.230169508576028E-4</v>
+      </c>
+      <c r="M16" s="35">
+        <f t="shared" si="2"/>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="3"/>
+        <v>0.33640000000000009</v>
+      </c>
+    </row>
+    <row r="17" spans="4:14" ht="15">
+      <c r="D17" s="48">
+        <v>14</v>
+      </c>
+      <c r="E17" s="35">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="F17" s="35">
+        <v>11.4</v>
+      </c>
+      <c r="G17" s="35">
+        <v>0.78</v>
+      </c>
+      <c r="H17" s="35">
+        <v>1.1240000000000001</v>
+      </c>
+      <c r="I17" s="35">
+        <v>11.4</v>
+      </c>
+      <c r="J17" s="35">
+        <v>13.7</v>
+      </c>
+      <c r="K17" s="35">
+        <f t="shared" si="0"/>
+        <v>5.248226950354605E-2</v>
+      </c>
+      <c r="L17" s="50">
+        <f t="shared" si="1"/>
+        <v>2.7543886122428397E-3</v>
+      </c>
+      <c r="M17" s="35">
+        <f t="shared" si="2"/>
+        <v>1.4799999999999986</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="3"/>
+        <v>2.1903999999999959</v>
+      </c>
+    </row>
+    <row r="18" spans="4:14" ht="15">
+      <c r="D18" s="48">
+        <v>15</v>
+      </c>
+      <c r="E18" s="35">
+        <v>9.5</v>
+      </c>
+      <c r="F18" s="35">
+        <v>9</v>
+      </c>
+      <c r="G18" s="35">
+        <v>0.74</v>
+      </c>
+      <c r="H18" s="35">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="I18" s="35">
+        <v>9</v>
+      </c>
+      <c r="J18" s="35">
+        <v>14.1</v>
+      </c>
+      <c r="K18" s="35">
+        <f t="shared" si="0"/>
+        <v>6.6666666666666638E-2</v>
+      </c>
+      <c r="L18" s="50">
+        <f t="shared" si="1"/>
+        <v>4.444444444444441E-3</v>
+      </c>
+      <c r="M18" s="35">
+        <f t="shared" si="2"/>
+        <v>1.879999999999999</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="3"/>
+        <v>3.5343999999999962</v>
+      </c>
+    </row>
+    <row r="19" spans="4:14" ht="15">
+      <c r="D19" s="48">
+        <v>16</v>
+      </c>
+      <c r="E19" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="F19" s="35">
+        <v>1</v>
+      </c>
+      <c r="G19" s="35">
+        <v>0.13</v>
+      </c>
+      <c r="H19" s="35">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="I19" s="35">
+        <v>1</v>
+      </c>
+      <c r="J19" s="35">
+        <v>14.5</v>
+      </c>
+      <c r="K19" s="35">
+        <f t="shared" si="0"/>
+        <v>8.0851063829787212E-2</v>
+      </c>
+      <c r="L19" s="50">
+        <f t="shared" si="1"/>
+        <v>6.5368945224083264E-3</v>
+      </c>
+      <c r="M19" s="35">
+        <f t="shared" si="2"/>
+        <v>2.2799999999999994</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="3"/>
+        <v>5.1983999999999968</v>
+      </c>
+    </row>
+    <row r="20" spans="4:14" ht="15">
+      <c r="D20" s="48">
+        <v>17</v>
+      </c>
+      <c r="E20" s="35">
+        <v>18.5</v>
+      </c>
+      <c r="F20" s="35">
+        <v>17</v>
+      </c>
+      <c r="G20" s="35">
+        <v>1.26</v>
+      </c>
+      <c r="H20" s="35">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="I20" s="35">
+        <v>17</v>
+      </c>
+      <c r="J20" s="35">
+        <v>14.9</v>
+      </c>
+      <c r="K20" s="35">
+        <f t="shared" si="0"/>
+        <v>9.50354609929078E-2</v>
+      </c>
+      <c r="L20" s="50">
+        <f t="shared" si="1"/>
+        <v>9.0317388461345002E-3</v>
+      </c>
+      <c r="M20" s="35">
+        <f t="shared" si="2"/>
+        <v>2.6799999999999997</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="3"/>
+        <v>7.1823999999999986</v>
+      </c>
+    </row>
+    <row r="21" spans="4:14" ht="15">
+      <c r="D21" s="48">
+        <v>18</v>
+      </c>
+      <c r="E21" s="35">
+        <v>12.6</v>
+      </c>
+      <c r="F21" s="35">
+        <v>12.8</v>
+      </c>
+      <c r="G21" s="35">
+        <v>1.08</v>
+      </c>
+      <c r="H21" s="35">
+        <v>1.0389999999999999</v>
+      </c>
+      <c r="I21" s="35">
+        <v>12.8</v>
+      </c>
+      <c r="J21" s="35">
+        <v>15</v>
+      </c>
+      <c r="K21" s="35">
+        <f t="shared" si="0"/>
+        <v>9.8581560283687919E-2</v>
+      </c>
+      <c r="L21" s="50">
+        <f t="shared" si="1"/>
+        <v>9.7183240279663952E-3</v>
+      </c>
+      <c r="M21" s="35">
+        <f t="shared" si="2"/>
+        <v>2.7799999999999994</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="3"/>
+        <v>7.7283999999999962</v>
+      </c>
+    </row>
+    <row r="22" spans="4:14" ht="15">
+      <c r="D22" s="48">
+        <v>19</v>
+      </c>
+      <c r="E22" s="35">
+        <v>17.5</v>
+      </c>
+      <c r="F22" s="35">
+        <v>15.8</v>
+      </c>
+      <c r="G22" s="35">
+        <v>0.96</v>
+      </c>
+      <c r="H22" s="35">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="I22" s="35">
+        <v>15.8</v>
+      </c>
+      <c r="J22" s="35">
+        <v>15.1</v>
+      </c>
+      <c r="K22" s="35">
+        <f t="shared" si="0"/>
+        <v>0.10212765957446805</v>
+      </c>
+      <c r="L22" s="50">
+        <f t="shared" si="1"/>
+        <v>1.0430058850158436E-2</v>
+      </c>
+      <c r="M22" s="35">
+        <f t="shared" si="2"/>
+        <v>2.879999999999999</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="3"/>
+        <v>8.2943999999999942</v>
+      </c>
+    </row>
+    <row r="23" spans="4:14" ht="15">
+      <c r="D23" s="48">
+        <v>20</v>
+      </c>
+      <c r="E23" s="35">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F23" s="35">
+        <v>4.5</v>
+      </c>
+      <c r="G23" s="35">
+        <v>0.42</v>
+      </c>
+      <c r="H23" s="35">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="I23" s="35">
+        <v>4.5</v>
+      </c>
+      <c r="J23" s="35">
+        <v>15.2</v>
+      </c>
+      <c r="K23" s="35">
+        <f t="shared" si="0"/>
+        <v>0.10567375886524819</v>
+      </c>
+      <c r="L23" s="50">
+        <f t="shared" si="1"/>
+        <v>1.116694331271062E-2</v>
+      </c>
+      <c r="M23" s="35">
+        <f t="shared" si="2"/>
+        <v>2.9799999999999986</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="3"/>
+        <v>8.8803999999999927</v>
+      </c>
+    </row>
+    <row r="24" spans="4:14" ht="15">
+      <c r="D24" s="48">
+        <v>21</v>
+      </c>
+      <c r="E24" s="35">
+        <v>15.9</v>
+      </c>
+      <c r="F24" s="35">
+        <v>14.5</v>
+      </c>
+      <c r="G24" s="35">
+        <v>1.01</v>
+      </c>
+      <c r="H24" s="35">
+        <v>1</v>
+      </c>
+      <c r="I24" s="35">
+        <v>14.5</v>
+      </c>
+      <c r="J24" s="35">
+        <v>15.8</v>
+      </c>
+      <c r="K24" s="35">
+        <f t="shared" si="0"/>
+        <v>0.12695035460992909</v>
+      </c>
+      <c r="L24" s="50">
+        <f t="shared" si="1"/>
+        <v>1.6116392535586745E-2</v>
+      </c>
+      <c r="M24" s="35">
+        <f t="shared" si="2"/>
+        <v>3.58</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="3"/>
+        <v>12.8164</v>
+      </c>
+    </row>
+    <row r="25" spans="4:14" ht="15">
+      <c r="D25" s="48">
+        <v>22</v>
+      </c>
+      <c r="E25" s="35">
+        <v>8.5</v>
+      </c>
+      <c r="F25" s="35">
+        <v>7.3</v>
+      </c>
+      <c r="G25" s="35">
+        <v>0.61</v>
+      </c>
+      <c r="H25" s="35">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="I25" s="35">
+        <v>7.3</v>
+      </c>
+      <c r="J25" s="35">
+        <v>16</v>
+      </c>
+      <c r="K25" s="35">
+        <f t="shared" si="0"/>
+        <v>0.13404255319148933</v>
+      </c>
+      <c r="L25" s="50">
+        <f t="shared" si="1"/>
+        <v>1.7967406066093247E-2</v>
+      </c>
+      <c r="M25" s="35">
+        <f t="shared" si="2"/>
+        <v>3.7799999999999994</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="3"/>
+        <v>14.288399999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="4:14" ht="15">
+      <c r="D26" s="48">
+        <v>23</v>
+      </c>
+      <c r="E26" s="35">
+        <v>10.6</v>
+      </c>
+      <c r="F26" s="35">
+        <v>8.6</v>
+      </c>
+      <c r="G26" s="35">
+        <v>0.69</v>
+      </c>
+      <c r="H26" s="35">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="I26" s="35">
+        <v>8.6</v>
+      </c>
+      <c r="J26" s="35">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="K26" s="35">
+        <f t="shared" si="0"/>
+        <v>0.15531914893617024</v>
+      </c>
+      <c r="L26" s="50">
+        <f t="shared" si="1"/>
+        <v>2.4124038026256234E-2</v>
+      </c>
+      <c r="M26" s="35">
+        <f t="shared" si="2"/>
+        <v>4.3800000000000008</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="3"/>
+        <v>19.184400000000007</v>
+      </c>
+    </row>
+    <row r="27" spans="4:14" ht="15">
+      <c r="D27" s="48">
+        <v>24</v>
+      </c>
+      <c r="E27" s="35">
+        <v>13.9</v>
+      </c>
+      <c r="F27" s="35">
+        <v>15.2</v>
+      </c>
+      <c r="G27" s="35">
+        <v>1.02</v>
+      </c>
+      <c r="H27" s="35">
+        <v>0.95</v>
+      </c>
+      <c r="I27" s="35">
+        <v>15.2</v>
+      </c>
+      <c r="J27" s="35">
+        <v>17</v>
+      </c>
+      <c r="K27" s="35">
+        <f t="shared" si="0"/>
+        <v>0.16950354609929077</v>
+      </c>
+      <c r="L27" s="50">
+        <f t="shared" si="1"/>
+        <v>2.8731452140234395E-2</v>
+      </c>
+      <c r="M27" s="35">
+        <f t="shared" si="2"/>
+        <v>4.7799999999999994</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="3"/>
+        <v>22.848399999999994</v>
+      </c>
+    </row>
+    <row r="28" spans="4:14" ht="15">
+      <c r="D28" s="48">
+        <v>25</v>
+      </c>
+      <c r="E28" s="35">
+        <v>14.9</v>
+      </c>
+      <c r="F28" s="35">
+        <v>12</v>
+      </c>
+      <c r="G28" s="35">
+        <v>0.82</v>
+      </c>
+      <c r="H28" s="35">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="I28" s="35">
+        <v>12</v>
+      </c>
+      <c r="J28" s="35">
+        <v>29.8</v>
+      </c>
+      <c r="K28" s="35">
+        <f t="shared" si="0"/>
+        <v>0.62340425531914889</v>
+      </c>
+      <c r="L28" s="50">
+        <f t="shared" si="1"/>
+        <v>0.38863286555002258</v>
+      </c>
+      <c r="M28" s="35">
+        <f t="shared" si="2"/>
+        <v>17.579999999999998</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="3"/>
+        <v>309.05639999999994</v>
+      </c>
+    </row>
+    <row r="30" spans="4:14" ht="15">
+      <c r="I30" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="J30" s="34">
+        <f>AVERAGE(J4:J28)</f>
+        <v>12.216000000000001</v>
+      </c>
+      <c r="K30" s="34">
+        <f>AVERAGE(K4:K28)</f>
+        <v>-1.4184397163123917E-4</v>
+      </c>
+      <c r="N30">
+        <f>SUM(N4:N28)</f>
+        <v>770.43399999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="4:14" ht="15">
+      <c r="H31" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="I31" s="49"/>
+      <c r="J31" s="35">
+        <f>SUM(J28-J4)</f>
+        <v>28.8</v>
+      </c>
+      <c r="K31" s="51">
+        <f>SUM(K28-K4)</f>
+        <v>1.0212765957446808</v>
+      </c>
+      <c r="L31" s="52"/>
+      <c r="M31" s="52"/>
+      <c r="N31" s="52">
+        <f>SUM(N30/25)</f>
+        <v>30.817359999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="J4:J28">
+    <sortCondition ref="J4"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="H31:I31"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>